<commit_message>
Figures new and table modified
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="lattice" sheetId="1" r:id="rId1"/>
     <sheet name="para_cbox" sheetId="2" r:id="rId2"/>
     <sheet name="para_eccen" sheetId="3" r:id="rId3"/>
-    <sheet name="para_M" sheetId="4" r:id="rId4"/>
+    <sheet name="para_B" sheetId="6" r:id="rId4"/>
+    <sheet name="para_L" sheetId="7" r:id="rId5"/>
+    <sheet name="para_M" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="97">
   <si>
     <t xml:space="preserve">Number of unit cells in spanwise direction </t>
   </si>
@@ -305,6 +307,9 @@
   </si>
   <si>
     <t>Standard</t>
+  </si>
+  <si>
+    <t>equivForce</t>
   </si>
 </sst>
 </file>
@@ -381,6 +386,220 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_cbox!$F$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_cbox!$F$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>305.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>384.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>523.17999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>662.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="36371200"/>
+        <c:axId val="56747712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="36371200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Wing-box thickness (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="56747712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="56747712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="36371200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -438,11 +657,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114869952"/>
-        <c:axId val="114868800"/>
+        <c:axId val="52907392"/>
+        <c:axId val="52907968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114869952"/>
+        <c:axId val="52907392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,12 +671,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114868800"/>
+        <c:crossAx val="52907968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114868800"/>
+        <c:axId val="52907968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -468,7 +687,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114869952"/>
+        <c:crossAx val="52907392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -491,6 +710,41 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -950,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O102"/>
+  <dimension ref="A1:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,33 +1216,42 @@
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="C7">
         <v>-800</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7">
+        <v>-700</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1004,8 +1267,44 @@
       <c r="E8">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>0.6</v>
+      </c>
+      <c r="H8">
+        <v>0.7</v>
+      </c>
+      <c r="I8">
+        <v>0.8</v>
+      </c>
+      <c r="J8">
+        <v>0.9</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M8">
+        <v>1.2</v>
+      </c>
+      <c r="N8">
+        <v>1.3</v>
+      </c>
+      <c r="O8">
+        <v>1.4</v>
+      </c>
+      <c r="P8">
+        <v>1.5</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1021,8 +1320,44 @@
       <c r="E9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0.32</v>
+      </c>
+      <c r="G9">
+        <v>0.436</v>
+      </c>
+      <c r="H9">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I9">
+        <v>0.74739999999999995</v>
+      </c>
+      <c r="J9">
+        <v>0.94579999999999997</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1038,26 +1373,52 @@
       <c r="E10" s="1">
         <v>2E-8</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O11" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11">
+        <f>F9*ABS($G$7)</f>
+        <v>224</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:J11" si="0">G9*ABS($G$7)</f>
+        <v>305.2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>384.3</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>523.17999999999995</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>662.06</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1073,11 +1434,11 @@
       <c r="E14" t="s">
         <v>35</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S14" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.8</v>
       </c>
@@ -1093,11 +1454,11 @@
       <c r="E15">
         <v>-10.067</v>
       </c>
-      <c r="O15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S15" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1113,11 +1474,11 @@
       <c r="E16">
         <v>-11.316000000000001</v>
       </c>
-      <c r="O16" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.2</v>
       </c>
@@ -1133,11 +1494,11 @@
       <c r="E17">
         <v>-12.16</v>
       </c>
-      <c r="O17" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.4</v>
       </c>
@@ -1153,24 +1514,24 @@
       <c r="E18">
         <v>-14.06</v>
       </c>
-      <c r="O18" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O19" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S18" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="O20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1192,11 +1553,11 @@
       <c r="G21" t="s">
         <v>41</v>
       </c>
-      <c r="O21" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S21" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.8</v>
       </c>
@@ -1218,11 +1579,11 @@
       <c r="G22">
         <v>0.33400000000000002</v>
       </c>
-      <c r="O22" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S22" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1244,11 +1605,11 @@
       <c r="G23">
         <v>0.97099999999999997</v>
       </c>
-      <c r="O23" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1.2</v>
       </c>
@@ -1270,11 +1631,11 @@
       <c r="G24">
         <v>0.97099999999999997</v>
       </c>
-      <c r="O24" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S24" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1.4</v>
       </c>
@@ -1296,397 +1657,378 @@
       <c r="G25">
         <v>0.97099999999999997</v>
       </c>
-      <c r="O25" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O26" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O27" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O28" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O29" s="2" t="s">
+      <c r="S25" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O30" s="2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S26" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O31" s="2" t="s">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S27" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O32" s="2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S28" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O33" s="2" t="s">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S29" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O34" s="2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S30" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O35" s="2" t="s">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O36" s="2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S32" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O37" s="2" t="s">
+    <row r="33" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S33" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O38" s="2">
+    <row r="34" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S34" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O39" s="2" t="s">
+    <row r="35" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S35" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O40" s="2">
+    <row r="36" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S36" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O41" s="2" t="s">
+    <row r="37" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S37" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O42" s="2">
+    <row r="38" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S38" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O43" s="2" t="s">
+    <row r="39" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S39" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O44" s="2" t="s">
+    <row r="40" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S40" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O45" s="2" t="s">
+    <row r="41" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S41" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O46" s="2" t="s">
+    <row r="42" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S42" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O47" s="2" t="s">
+    <row r="43" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S43" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O48" s="2">
+    <row r="44" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S44" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O49" s="2" t="s">
+    <row r="45" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S45" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O50" s="2">
+    <row r="46" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S46" s="2">
         <v>300</v>
       </c>
     </row>
-    <row r="51" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O51" s="2" t="s">
+    <row r="47" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S47" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O52" s="2">
+    <row r="48" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S48" s="2">
         <v>713.86273190300005</v>
       </c>
     </row>
-    <row r="53" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O53" s="2" t="s">
+    <row r="49" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S49" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O54" s="2">
+    <row r="50" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S50" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row r="55" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O55" s="2" t="s">
+    <row r="51" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S51" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O56" s="2">
+    <row r="52" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S52" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O57" s="2" t="s">
+    <row r="53" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S53" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O58" s="2" t="s">
+    <row r="54" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S54" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O59" s="2" t="s">
+    <row r="55" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S55" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O60" s="2" t="s">
+    <row r="56" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S56" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O61" s="2" t="s">
+    <row r="57" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S57" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O62" s="2" t="s">
+    <row r="58" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S58" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O63" s="2" t="s">
+    <row r="59" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S59" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O64" s="2" t="s">
+    <row r="60" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S60" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O65" s="2" t="s">
+    <row r="61" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S61" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O66" s="2" t="s">
+    <row r="62" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S62" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O67" s="2" t="s">
+    <row r="63" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S63" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O68" s="2">
+    <row r="64" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S64" s="2">
         <v>-50</v>
       </c>
     </row>
-    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O69" s="2" t="s">
+    <row r="65" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S65" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O70" s="2">
+    <row r="66" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S66" s="2">
         <v>-800</v>
       </c>
     </row>
-    <row r="71" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O71" s="2" t="s">
+    <row r="67" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S67" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O72" s="2">
+    <row r="68" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S68" s="2">
         <v>-200000</v>
       </c>
     </row>
-    <row r="73" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O73" s="2" t="s">
+    <row r="69" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S69" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O74" s="2">
+    <row r="70" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S70" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="75" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O75" s="2" t="s">
+    <row r="71" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S71" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O76" s="2">
+    <row r="72" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S72" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O77" s="2" t="s">
+    <row r="73" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S73" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O78" s="2">
+    <row r="74" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S74" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O79" s="2" t="s">
+    <row r="75" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S75" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O80" s="2">
+    <row r="76" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S76" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="81" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O81" s="2" t="s">
+    <row r="77" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S77" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O82" s="2">
+    <row r="78" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S78" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O83" s="2" t="s">
+    <row r="79" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S79" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O84" s="2">
+    <row r="80" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S80" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O85" s="2" t="s">
+    <row r="81" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S81" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O86" s="2">
+    <row r="82" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S82" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="87" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O87" s="2" t="s">
+    <row r="83" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S83" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O88" s="2">
+    <row r="84" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S84" s="2">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="89" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O89" s="2" t="s">
+    <row r="85" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S85" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O90" s="3">
+    <row r="86" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S86" s="3">
         <v>1.0000000000000001E-15</v>
       </c>
     </row>
-    <row r="91" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O91" s="2" t="s">
+    <row r="87" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S87" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O92" s="2">
+    <row r="88" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S88" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="93" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O93" s="2" t="s">
+    <row r="89" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S89" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O94" s="2" t="b">
+    <row r="90" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S90" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O95" s="2" t="s">
+    <row r="91" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S91" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O96" s="2" t="b">
+    <row r="92" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S92" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O97" s="2" t="s">
+    <row r="93" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S93" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="98" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O98" s="3">
+    <row r="94" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S94" s="3">
         <v>2E-8</v>
       </c>
     </row>
-    <row r="99" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O99" s="2" t="s">
+    <row r="95" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S95" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O100" s="2" t="s">
+    <row r="96" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S96" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O101" s="2" t="s">
+    <row r="97" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S97" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="102" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O102" s="2" t="s">
+    <row r="98" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S98" s="2" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2439,7 +2781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -2654,4 +2996,314 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A7:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>-700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>-0.159</v>
+      </c>
+      <c r="C14">
+        <v>14.946999999999999</v>
+      </c>
+      <c r="D14">
+        <v>-0.126</v>
+      </c>
+      <c r="E14">
+        <v>-15.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>-10.946</v>
+      </c>
+      <c r="C15">
+        <v>13.666</v>
+      </c>
+      <c r="D15">
+        <v>-0.17499999999999999</v>
+      </c>
+      <c r="E15">
+        <v>-10.269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <v>-14.752000000000001</v>
+      </c>
+      <c r="C16">
+        <v>8.6950000000000003</v>
+      </c>
+      <c r="D16">
+        <v>-0.20799999999999999</v>
+      </c>
+      <c r="E16">
+        <v>-10.125999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E22">
+        <v>-0.999</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>50</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.121</v>
+      </c>
+      <c r="E23">
+        <v>-122.756</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.54600000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>70</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="E24">
+        <v>-99.478999999999999</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A7:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="B9:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>-700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
A lot of changes
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,22 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="lattice" sheetId="1" r:id="rId1"/>
     <sheet name="para_cbox" sheetId="2" r:id="rId2"/>
     <sheet name="para_eccen" sheetId="3" r:id="rId3"/>
-    <sheet name="para_B" sheetId="6" r:id="rId4"/>
-    <sheet name="para_L" sheetId="7" r:id="rId5"/>
-    <sheet name="para_M" sheetId="4" r:id="rId6"/>
+    <sheet name="para_B" sheetId="4" r:id="rId4"/>
+    <sheet name="para_M" sheetId="6" r:id="rId5"/>
+    <sheet name="para_N" sheetId="9" r:id="rId6"/>
+    <sheet name="para_L" sheetId="7" r:id="rId7"/>
+    <sheet name="para_chiral_t" sheetId="8" r:id="rId8"/>
+    <sheet name="para_r" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="103">
   <si>
     <t xml:space="preserve">Number of unit cells in spanwise direction </t>
   </si>
@@ -117,42 +120,12 @@
     <t>Parameter value</t>
   </si>
   <si>
-    <t>\phi_{\mathrm{max}}</t>
-  </si>
-  <si>
-    <t>e_{\phi,\mathrm{max}}</t>
-  </si>
-  <si>
-    <t>\tilde{\phi}_{\mathrm{max}}</t>
-  </si>
-  <si>
-    <t>e_{\tilde{\phi},\mathrm{max}}</t>
-  </si>
-  <si>
     <t>damp</t>
   </si>
   <si>
     <t>Vertical displacement U2 (mm)</t>
   </si>
   <si>
-    <t>v_{\mathrm{max}}</t>
-  </si>
-  <si>
-    <t>\hat{x}_{v_{\mathrm{max}}}</t>
-  </si>
-  <si>
-    <t>\hat{z}_{v_{\mathrm{max}}}</t>
-  </si>
-  <si>
-    <t>\hat{x}_{v_{\mathrm{min}}}</t>
-  </si>
-  <si>
-    <t>\hat{z}_{v_{\mathrm{min}}}</t>
-  </si>
-  <si>
-    <t>v_{\mathrm{min}}</t>
-  </si>
-  <si>
     <t>Iter</t>
   </si>
   <si>
@@ -310,6 +283,54 @@
   </si>
   <si>
     <t>equivForce</t>
+  </si>
+  <si>
+    <t>Delta:</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>no buckling</t>
+  </si>
+  <si>
+    <t>0.088-107.229</t>
+  </si>
+  <si>
+    <t>0.081-137.131</t>
+  </si>
+  <si>
+    <t>Wing-box height (mm)</t>
+  </si>
+  <si>
+    <t>$\phi_{\mathrm{max}}$</t>
+  </si>
+  <si>
+    <t>$e_{\phi,\mathrm{max}}$</t>
+  </si>
+  <si>
+    <t>$\tilde{\phi}_{\mathrm{max}}}$</t>
+  </si>
+  <si>
+    <t>$e_{\tilde{\phi},\mathrm{max}}$</t>
+  </si>
+  <si>
+    <t>$\hat{x}_{v_{\mathrm{max}}}$</t>
+  </si>
+  <si>
+    <t>$v_{\mathrm{min}}$</t>
+  </si>
+  <si>
+    <t>$\hat{z}_{v_{\mathrm{min}}}$</t>
+  </si>
+  <si>
+    <t>$\hat{x}_{v_{\mathrm{min}}}$</t>
+  </si>
+  <si>
+    <t>$v_{\mathrm{max}}$</t>
+  </si>
+  <si>
+    <t>$\hat{z}_{v_{\mathrm{max}}}$</t>
   </si>
 </sst>
 </file>
@@ -386,14 +407,16 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -403,16 +426,13 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
               </a:ln>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>para_cbox!$F$8:$J$8</c:f>
@@ -461,7 +481,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -471,11 +491,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="36371200"/>
-        <c:axId val="56747712"/>
+        <c:axId val="77918720"/>
+        <c:axId val="77919296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="36371200"/>
+        <c:axId val="77918720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -483,7 +503,11 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:minorGridlines/>
         <c:title>
           <c:tx>
@@ -518,12 +542,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56747712"/>
+        <c:crossAx val="77919296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56747712"/>
+        <c:axId val="77919296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200"/>
@@ -565,7 +589,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36371200"/>
+        <c:crossAx val="77918720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -657,11 +681,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="52907392"/>
-        <c:axId val="52907968"/>
+        <c:axId val="77921024"/>
+        <c:axId val="77921600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52907392"/>
+        <c:axId val="77921024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,12 +695,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52907968"/>
+        <c:crossAx val="77921600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52907968"/>
+        <c:axId val="77921600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,7 +711,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52907392"/>
+        <c:crossAx val="77921024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -709,20 +733,1036 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_N!$J$8:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>611.88229999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>713.86699999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>815.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>917.82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1019.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1121.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_N!$C$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>522.83000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>390.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>376.74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>333.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>303.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="84293824"/>
+        <c:axId val="84294400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="84293824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1100"/>
+          <c:min val="600"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Wing-box length</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>(mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84294400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="84294400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="600"/>
+          <c:min val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84293824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_chiral_t!$F$8:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_chiral_t!$F$10:$S$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>156.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>222.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>264.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>295.46999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>331.31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>476.84000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>456.40000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>544.53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>598.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>620.54999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>652.89</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>689.40199999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="84308480"/>
+        <c:axId val="94103808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="84308480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Chiral lattice</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> thickness </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>(mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94103808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="94103808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84308480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_chiral_t!$M$32:$M$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_chiral_t!$N$32:$N$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-5.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10.475</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.9169999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.247</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.4420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.3710000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.0330000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.379</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.3239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-7.1669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.1859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.9409999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.6120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-6.76</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.8230000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="94107840"/>
+        <c:axId val="94108992"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="94107840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Chiral lattice</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> thickness </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>(mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94108992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="94108992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1400">
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>ϕ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" sz="1400" baseline="-25000">
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>tip</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t> (deg)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94107840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_r!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_r!$B$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>477.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>523.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>552.44000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>546.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="94101504"/>
+        <c:axId val="94103232"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="94101504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Wing-box length</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>(mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94103232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="94103232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94101504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -763,6 +1803,149 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>312644</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>88526</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>312645</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>20171</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>312644</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1206,8 +2389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S98"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9:P9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,7 +2431,7 @@
         <v>-700</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1354,12 +2537,12 @@
         <v>28</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
         <v>2E-8</v>
@@ -1374,12 +2557,12 @@
         <v>2E-8</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F11">
         <f>F9*ABS($G$7)</f>
@@ -1402,12 +2585,12 @@
         <v>662.06</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S12" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1415,7 +2598,7 @@
         <v>29</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1423,16 +2606,28 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>96</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" t="s">
+        <v>100</v>
       </c>
       <c r="S14" s="2">
         <v>10</v>
@@ -1454,8 +2649,20 @@
       <c r="E15">
         <v>-10.067</v>
       </c>
+      <c r="F15">
+        <v>0.121</v>
+      </c>
+      <c r="G15">
+        <v>-16.908000000000001</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0.33400000000000002</v>
+      </c>
       <c r="S15" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1474,6 +2681,18 @@
       <c r="E16">
         <v>-11.316000000000001</v>
       </c>
+      <c r="F16">
+        <v>0.121</v>
+      </c>
+      <c r="G16">
+        <v>-1.292</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0.97099999999999997</v>
+      </c>
       <c r="S16" s="2">
         <v>1</v>
       </c>
@@ -1494,6 +2713,18 @@
       <c r="E17">
         <v>-12.16</v>
       </c>
+      <c r="F17">
+        <v>0.121</v>
+      </c>
+      <c r="G17">
+        <v>-1.081</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0.97099999999999997</v>
+      </c>
       <c r="S17" s="2" t="s">
         <v>2</v>
       </c>
@@ -1514,6 +2745,18 @@
       <c r="E18">
         <v>-14.06</v>
       </c>
+      <c r="F18">
+        <v>0.121</v>
+      </c>
+      <c r="G18">
+        <v>-0.95</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0.97099999999999997</v>
+      </c>
       <c r="S18" s="2">
         <v>8</v>
       </c>
@@ -1525,7 +2768,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="S20" s="2">
         <v>3</v>
@@ -1536,25 +2779,25 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
+        <v>100</v>
+      </c>
+      <c r="S21" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -1606,7 +2849,7 @@
         <v>0.97099999999999997</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -1658,7 +2901,7 @@
         <v>0.97099999999999997</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -1668,7 +2911,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S27" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -1678,7 +2921,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S29" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -1698,7 +2941,7 @@
     </row>
     <row r="33" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S33" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="19:19" x14ac:dyDescent="0.25">
@@ -1708,7 +2951,7 @@
     </row>
     <row r="35" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S35" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="19:19" x14ac:dyDescent="0.25">
@@ -1718,7 +2961,7 @@
     </row>
     <row r="37" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S37" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="19:19" x14ac:dyDescent="0.25">
@@ -1728,27 +2971,27 @@
     </row>
     <row r="39" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S39" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S40" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S41" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S42" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S43" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="19:19" x14ac:dyDescent="0.25">
@@ -1758,7 +3001,7 @@
     </row>
     <row r="45" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S45" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="19:19" x14ac:dyDescent="0.25">
@@ -1768,7 +3011,7 @@
     </row>
     <row r="47" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S47" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="19:19" x14ac:dyDescent="0.25">
@@ -1778,7 +3021,7 @@
     </row>
     <row r="49" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S49" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="19:19" x14ac:dyDescent="0.25">
@@ -1788,7 +3031,7 @@
     </row>
     <row r="51" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S51" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="19:19" x14ac:dyDescent="0.25">
@@ -1798,57 +3041,57 @@
     </row>
     <row r="53" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S53" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S54" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S55" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S56" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S57" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S58" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S59" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S60" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S61" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S62" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S63" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="19:19" x14ac:dyDescent="0.25">
@@ -1858,7 +3101,7 @@
     </row>
     <row r="65" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S65" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="19:19" x14ac:dyDescent="0.25">
@@ -1868,7 +3111,7 @@
     </row>
     <row r="67" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S67" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="19:19" x14ac:dyDescent="0.25">
@@ -1878,7 +3121,7 @@
     </row>
     <row r="69" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S69" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="19:19" x14ac:dyDescent="0.25">
@@ -1888,7 +3131,7 @@
     </row>
     <row r="71" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S71" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="19:19" x14ac:dyDescent="0.25">
@@ -1898,7 +3141,7 @@
     </row>
     <row r="73" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S73" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="19:19" x14ac:dyDescent="0.25">
@@ -1908,7 +3151,7 @@
     </row>
     <row r="75" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S75" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="19:19" x14ac:dyDescent="0.25">
@@ -1918,7 +3161,7 @@
     </row>
     <row r="77" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S77" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="19:19" x14ac:dyDescent="0.25">
@@ -1928,7 +3171,7 @@
     </row>
     <row r="79" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S79" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="19:19" x14ac:dyDescent="0.25">
@@ -1938,7 +3181,7 @@
     </row>
     <row r="81" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S81" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="19:19" x14ac:dyDescent="0.25">
@@ -1948,7 +3191,7 @@
     </row>
     <row r="83" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S83" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="84" spans="19:19" x14ac:dyDescent="0.25">
@@ -1958,7 +3201,7 @@
     </row>
     <row r="85" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S85" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="19:19" x14ac:dyDescent="0.25">
@@ -1968,7 +3211,7 @@
     </row>
     <row r="87" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S87" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="19:19" x14ac:dyDescent="0.25">
@@ -1978,7 +3221,7 @@
     </row>
     <row r="89" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S89" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="90" spans="19:19" x14ac:dyDescent="0.25">
@@ -1988,7 +3231,7 @@
     </row>
     <row r="91" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S91" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="92" spans="19:19" x14ac:dyDescent="0.25">
@@ -1998,7 +3241,7 @@
     </row>
     <row r="93" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S93" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="19:19" x14ac:dyDescent="0.25">
@@ -2008,22 +3251,22 @@
     </row>
     <row r="95" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S95" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="96" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S96" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S97" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="98" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S98" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2055,7 +3298,7 @@
         <v>24</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -2068,12 +3311,12 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R4" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R5" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2084,7 +3327,7 @@
         <v>-700</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2107,7 +3350,7 @@
         <v>0.01</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2130,7 +3373,7 @@
         <v>28</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2140,7 +3383,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R10" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2156,16 +3399,16 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>2</v>
@@ -2248,7 +3491,7 @@
         <v>-10.598000000000001</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2273,12 +3516,12 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R18" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="R19" s="2">
         <v>20</v>
@@ -2289,25 +3532,25 @@
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="E20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" t="s">
+        <v>100</v>
+      </c>
+      <c r="R20" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="F20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" t="s">
-        <v>41</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2359,7 +3602,7 @@
         <v>0.33400000000000002</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2411,7 +3654,7 @@
         <v>0.33400000000000002</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2443,7 +3686,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R28" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2453,7 +3696,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R30" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2463,7 +3706,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R32" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="18:18" x14ac:dyDescent="0.25">
@@ -2473,27 +3716,27 @@
     </row>
     <row r="34" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R34" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R35" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R36" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R37" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R38" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="18:18" x14ac:dyDescent="0.25">
@@ -2503,7 +3746,7 @@
     </row>
     <row r="40" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R40" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="18:18" x14ac:dyDescent="0.25">
@@ -2513,7 +3756,7 @@
     </row>
     <row r="42" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R42" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="18:18" x14ac:dyDescent="0.25">
@@ -2523,7 +3766,7 @@
     </row>
     <row r="44" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R44" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="18:18" x14ac:dyDescent="0.25">
@@ -2533,7 +3776,7 @@
     </row>
     <row r="46" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R46" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="18:18" x14ac:dyDescent="0.25">
@@ -2543,57 +3786,57 @@
     </row>
     <row r="48" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R48" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R49" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R50" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R51" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R52" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R53" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R54" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R55" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R56" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R57" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R58" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="18:18" x14ac:dyDescent="0.25">
@@ -2603,7 +3846,7 @@
     </row>
     <row r="60" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R60" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="18:18" x14ac:dyDescent="0.25">
@@ -2613,7 +3856,7 @@
     </row>
     <row r="62" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R62" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="18:18" x14ac:dyDescent="0.25">
@@ -2623,7 +3866,7 @@
     </row>
     <row r="64" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R64" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="18:18" x14ac:dyDescent="0.25">
@@ -2633,7 +3876,7 @@
     </row>
     <row r="66" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R66" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="18:18" x14ac:dyDescent="0.25">
@@ -2643,7 +3886,7 @@
     </row>
     <row r="68" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R68" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="18:18" x14ac:dyDescent="0.25">
@@ -2653,7 +3896,7 @@
     </row>
     <row r="70" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R70" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="18:18" x14ac:dyDescent="0.25">
@@ -2663,7 +3906,7 @@
     </row>
     <row r="72" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R72" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="18:18" x14ac:dyDescent="0.25">
@@ -2673,7 +3916,7 @@
     </row>
     <row r="74" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R74" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="18:18" x14ac:dyDescent="0.25">
@@ -2683,7 +3926,7 @@
     </row>
     <row r="76" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R76" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="18:18" x14ac:dyDescent="0.25">
@@ -2693,7 +3936,7 @@
     </row>
     <row r="78" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R78" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="18:18" x14ac:dyDescent="0.25">
@@ -2703,7 +3946,7 @@
     </row>
     <row r="80" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R80" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="18:18" x14ac:dyDescent="0.25">
@@ -2713,7 +3956,7 @@
     </row>
     <row r="82" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R82" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="18:18" x14ac:dyDescent="0.25">
@@ -2723,7 +3966,7 @@
     </row>
     <row r="84" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R84" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="18:18" x14ac:dyDescent="0.25">
@@ -2733,7 +3976,7 @@
     </row>
     <row r="86" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R86" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="18:18" x14ac:dyDescent="0.25">
@@ -2743,7 +3986,7 @@
     </row>
     <row r="88" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R88" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89" spans="18:18" x14ac:dyDescent="0.25">
@@ -2753,22 +3996,22 @@
     </row>
     <row r="90" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R90" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="91" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R91" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R92" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R93" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2782,10 +4025,13 @@
   <dimension ref="A7:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -2800,13 +4046,13 @@
         <v>25</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2814,13 +4060,13 @@
         <v>26</v>
       </c>
       <c r="B9">
-        <v>0.74339999999999995</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
+        <v>0.61850000000000005</v>
+      </c>
+      <c r="C9">
+        <v>0.74619999999999997</v>
+      </c>
+      <c r="D9">
+        <v>0.85980000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2833,72 +4079,72 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B14">
-        <v>-0.877</v>
+        <v>-1.0820000000000001</v>
       </c>
       <c r="C14">
-        <v>9.5250000000000004</v>
+        <v>9.61</v>
       </c>
       <c r="D14">
-        <v>-0.17</v>
+        <v>-0.187</v>
       </c>
       <c r="E14">
-        <v>-10.196</v>
+        <v>-10.614000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B15">
-        <v>-0.13700000000000001</v>
+        <v>-0.877</v>
       </c>
       <c r="C15">
-        <v>22.16</v>
+        <v>9.5250000000000004</v>
       </c>
       <c r="D15">
-        <v>-0.104</v>
+        <v>-0.17</v>
       </c>
       <c r="E15">
-        <v>-10.448</v>
+        <v>-10.196</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B16">
-        <v>-0.877</v>
+        <v>-0.71</v>
       </c>
       <c r="C16">
-        <v>9.5250000000000004</v>
+        <v>9.5280000000000005</v>
       </c>
       <c r="D16">
-        <v>-0.17</v>
+        <v>-0.16</v>
       </c>
       <c r="E16">
-        <v>-10.196</v>
+        <v>-9.8379999999999992</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2906,39 +4152,39 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D22">
-        <v>0.121</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="E22">
-        <v>-9.8309999999999995</v>
+        <v>-10.941000000000001</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -2949,7 +4195,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2961,18 +4207,18 @@
         <v>0.121</v>
       </c>
       <c r="E23">
-        <v>-0.83099999999999996</v>
+        <v>-9.8309999999999995</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23">
-        <v>0.97099999999999997</v>
+        <v>0.33400000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2984,13 +4230,13 @@
         <v>0.121</v>
       </c>
       <c r="E24">
-        <v>-0.68500000000000005</v>
+        <v>-8.75</v>
       </c>
       <c r="F24">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>0.97099999999999997</v>
+        <v>0.33400000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -3000,9 +4246,698 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A7:N24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>-700</v>
+      </c>
+      <c r="E7">
+        <v>-1000</v>
+      </c>
+      <c r="L7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>0.74339999999999995</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>0.49509999999999998</v>
+      </c>
+      <c r="F9">
+        <v>0.85960000000000003</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9">
+        <v>353.27</v>
+      </c>
+      <c r="M9">
+        <v>529.90599999999995</v>
+      </c>
+      <c r="N9">
+        <v>706.54100000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>B9*ABS($C$7)</f>
+        <v>520.38</v>
+      </c>
+      <c r="C10" t="e">
+        <f t="shared" ref="C10:G10" si="0">C9*ABS($C$7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D10" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>346.57</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>601.72</v>
+      </c>
+      <c r="G10" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>-5.1790000000000003</v>
+      </c>
+      <c r="C14">
+        <v>13.558999999999999</v>
+      </c>
+      <c r="D14">
+        <v>-0.245</v>
+      </c>
+      <c r="E14">
+        <v>-10.074</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>-0.39200000000000002</v>
+      </c>
+      <c r="C15">
+        <v>22.16</v>
+      </c>
+      <c r="D15">
+        <v>-0.14799999999999999</v>
+      </c>
+      <c r="E15">
+        <v>-10.446999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>-0.214</v>
+      </c>
+      <c r="C16">
+        <v>14.893000000000001</v>
+      </c>
+      <c r="D16">
+        <v>-0.16400000000000001</v>
+      </c>
+      <c r="E16">
+        <v>-17.526</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.121</v>
+      </c>
+      <c r="E22">
+        <v>-29.166</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.121</v>
+      </c>
+      <c r="E23">
+        <v>-6.093</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.121</v>
+      </c>
+      <c r="E24">
+        <v>-1.018</v>
+      </c>
+      <c r="F24">
+        <v>0.6</v>
+      </c>
+      <c r="G24">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A7:O27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>700</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>611.88229999999999</v>
+      </c>
+      <c r="K8">
+        <v>713.86699999999996</v>
+      </c>
+      <c r="L8">
+        <v>815.84</v>
+      </c>
+      <c r="M8">
+        <v>917.82</v>
+      </c>
+      <c r="N8">
+        <v>1019.8</v>
+      </c>
+      <c r="O8">
+        <v>1121.78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>0.74690000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.55789999999999995</v>
+      </c>
+      <c r="E9">
+        <v>0.53820000000000001</v>
+      </c>
+      <c r="F9">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="G9">
+        <v>0.43419999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f>C9*$C$7</f>
+        <v>522.83000000000004</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:G10" si="0">D9*$C$7</f>
+        <v>390.53</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>376.74</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>333.2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>303.94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>-0.185</v>
+      </c>
+      <c r="C14">
+        <v>16.474</v>
+      </c>
+      <c r="D14">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="E14">
+        <v>-12.506</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>-0.878</v>
+      </c>
+      <c r="C15">
+        <v>9.5169999999999995</v>
+      </c>
+      <c r="D15">
+        <v>-0.17</v>
+      </c>
+      <c r="E15">
+        <v>-10.196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>-4.5819999999999999</v>
+      </c>
+      <c r="C16">
+        <v>11.090999999999999</v>
+      </c>
+      <c r="D16">
+        <v>-0.20899999999999999</v>
+      </c>
+      <c r="E16">
+        <v>-7.8479999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>-8.1159999999999997</v>
+      </c>
+      <c r="C17">
+        <v>6.1920000000000002</v>
+      </c>
+      <c r="D17">
+        <v>-0.248</v>
+      </c>
+      <c r="E17">
+        <v>-6.3979999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>-17.658999999999999</v>
+      </c>
+      <c r="C18">
+        <v>4.9539999999999997</v>
+      </c>
+      <c r="D18">
+        <v>-0.29899999999999999</v>
+      </c>
+      <c r="E18">
+        <v>-5.0979999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>-22.007000000000001</v>
+      </c>
+      <c r="C19">
+        <v>6.5270000000000001</v>
+      </c>
+      <c r="D19">
+        <v>-0.33700000000000002</v>
+      </c>
+      <c r="E19">
+        <v>-3.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="E22">
+        <v>-1.0609999999999999</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.121</v>
+      </c>
+      <c r="E23">
+        <v>-9.8439999999999994</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.108</v>
+      </c>
+      <c r="E24">
+        <v>-25.780999999999999</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="E25">
+        <v>-46.636000000000003</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
@@ -3051,16 +4986,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3116,7 +5051,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3124,22 +5059,22 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3216,68 +5151,961 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:G21"/>
+  <dimension ref="A7:V46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="B9:E9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="C7">
         <v>-700</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7">
+        <v>700</v>
+      </c>
+      <c r="L7" t="s">
+        <v>88</v>
+      </c>
+      <c r="N7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7" t="s">
+        <v>88</v>
+      </c>
+      <c r="V7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>0.2</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>0.4</v>
       </c>
       <c r="D8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="E8">
+        <v>0.8</v>
+      </c>
+      <c r="F8">
+        <v>0.05</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>0.15</v>
+      </c>
+      <c r="I8">
+        <v>0.2</v>
+      </c>
+      <c r="J8">
+        <v>0.25</v>
+      </c>
+      <c r="K8">
+        <v>0.3</v>
+      </c>
+      <c r="L8">
+        <v>0.35</v>
+      </c>
+      <c r="M8">
+        <v>0.4</v>
+      </c>
+      <c r="N8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O8">
+        <v>0.6</v>
+      </c>
+      <c r="P8">
+        <v>0.7</v>
+      </c>
+      <c r="Q8">
+        <v>0.8</v>
+      </c>
+      <c r="R8">
+        <v>0.85</v>
+      </c>
+      <c r="S8">
+        <v>0.9</v>
+      </c>
+      <c r="V8">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.49559999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.65429999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.84179999999999999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>0.18</v>
+      </c>
+      <c r="G9">
+        <v>0.223</v>
+      </c>
+      <c r="H9">
+        <v>0.28639999999999999</v>
+      </c>
+      <c r="I9">
+        <v>0.3175</v>
+      </c>
+      <c r="J9">
+        <v>0.37740000000000001</v>
+      </c>
+      <c r="K9">
+        <v>0.42209999999999998</v>
+      </c>
+      <c r="L9">
+        <v>0.4733</v>
+      </c>
+      <c r="M9">
+        <v>0.68120000000000003</v>
+      </c>
+      <c r="N9">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="O9">
+        <v>0.77790000000000004</v>
+      </c>
+      <c r="P9">
+        <v>0.85570000000000002</v>
+      </c>
+      <c r="Q9">
+        <v>0.88649999999999995</v>
+      </c>
+      <c r="R9">
+        <v>0.93269999999999997</v>
+      </c>
+      <c r="S9">
+        <v>0.98485999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>F9*$G$7</f>
+        <v>126</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:S10" si="0">G9*$G$7</f>
+        <v>156.1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>200.48</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>222.25</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>264.18</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>295.46999999999997</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>331.31</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>476.84000000000003</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>456.40000000000003</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>544.53</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>598.99</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>620.54999999999995</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>652.89</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>689.40199999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.2</v>
+      </c>
+      <c r="B14">
+        <v>-1.2010000000000001</v>
+      </c>
+      <c r="C14">
+        <v>9.4640000000000004</v>
+      </c>
+      <c r="D14">
+        <v>-0.19900000000000001</v>
+      </c>
+      <c r="E14">
+        <v>-10.637</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.4</v>
+      </c>
+      <c r="B15">
+        <v>-1.026</v>
+      </c>
+      <c r="C15">
+        <v>9.5030000000000001</v>
+      </c>
+      <c r="D15">
+        <v>-0.17899999999999999</v>
+      </c>
+      <c r="E15">
+        <v>-10.334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.6</v>
+      </c>
+      <c r="B16">
+        <v>-0.92200000000000004</v>
+      </c>
+      <c r="C16">
+        <v>13.874000000000001</v>
+      </c>
+      <c r="D16">
+        <v>-0.16400000000000001</v>
+      </c>
+      <c r="E16">
+        <v>-9.8160000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.8</v>
+      </c>
+      <c r="B17">
+        <v>-0.23200000000000001</v>
+      </c>
+      <c r="C17">
+        <v>14.445</v>
+      </c>
+      <c r="D17">
+        <v>-0.15</v>
+      </c>
+      <c r="E17">
+        <v>-9.3230000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.2</v>
+      </c>
+      <c r="B22">
+        <v>2.87</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="E22">
+        <v>-11.878</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.4</v>
+      </c>
+      <c r="B23">
+        <v>0.67</v>
+      </c>
+      <c r="C23">
+        <v>0.6</v>
+      </c>
+      <c r="D23">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="E23">
+        <v>-10.896000000000001</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.6</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0.05</v>
+      </c>
+      <c r="D24">
+        <v>0.121</v>
+      </c>
+      <c r="E24">
+        <v>-10.036</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.8</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.121</v>
+      </c>
+      <c r="E25">
+        <v>-1.4490000000000001</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>56</v>
+      </c>
+      <c r="M32">
+        <v>0.05</v>
+      </c>
+      <c r="N32">
+        <v>-5.35</v>
+      </c>
+      <c r="O32">
+        <v>14.167</v>
+      </c>
+      <c r="P32">
+        <v>-0.19</v>
+      </c>
+      <c r="Q32">
+        <v>-4.3029999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>56</v>
+      </c>
+      <c r="M33">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N33">
+        <v>-10.475</v>
+      </c>
+      <c r="O33">
+        <v>13.824999999999999</v>
+      </c>
+      <c r="P33">
+        <v>-0.17100000000000001</v>
+      </c>
+      <c r="Q33">
+        <v>-10.151999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34">
+        <v>0.6</v>
+      </c>
+      <c r="N34">
+        <v>-4.9169999999999998</v>
+      </c>
+      <c r="O34">
+        <v>9.7850000000000001</v>
+      </c>
+      <c r="P34">
+        <v>-0.16500000000000001</v>
+      </c>
+      <c r="Q34">
+        <v>-10.590999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>56</v>
+      </c>
+      <c r="M35">
+        <v>0.65</v>
+      </c>
+      <c r="N35">
+        <v>-0.247</v>
+      </c>
+      <c r="O35">
+        <v>9.8059999999999992</v>
+      </c>
+      <c r="P35">
+        <v>-0.16200000000000001</v>
+      </c>
+      <c r="Q35">
+        <v>-10.54</v>
+      </c>
+    </row>
+    <row r="36" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>56</v>
+      </c>
+      <c r="M36">
+        <v>0.7</v>
+      </c>
+      <c r="N36">
+        <v>-3.4420000000000002</v>
+      </c>
+      <c r="O36">
+        <v>9.827</v>
+      </c>
+      <c r="P36">
+        <v>-0.158</v>
+      </c>
+      <c r="Q36">
+        <v>-10.491</v>
+      </c>
+    </row>
+    <row r="37" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>56</v>
+      </c>
+      <c r="M37">
+        <v>0.8</v>
+      </c>
+      <c r="N37">
+        <v>-5.3710000000000004</v>
+      </c>
+      <c r="O37">
+        <v>14.603</v>
+      </c>
+      <c r="P37">
+        <v>-0.153</v>
+      </c>
+      <c r="Q37">
+        <v>-9.5739999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>56</v>
+      </c>
+      <c r="M38">
+        <v>0.85</v>
+      </c>
+      <c r="N38">
+        <v>-4.0330000000000004</v>
+      </c>
+      <c r="O38">
+        <v>14.756</v>
+      </c>
+      <c r="P38">
+        <v>-0.15</v>
+      </c>
+      <c r="Q38">
+        <v>-9.4610000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>56</v>
+      </c>
+      <c r="M39">
+        <v>0.9</v>
+      </c>
+      <c r="N39">
+        <v>-0.379</v>
+      </c>
+      <c r="O39">
+        <v>14.906000000000001</v>
+      </c>
+      <c r="P39">
+        <v>-0.14699999999999999</v>
+      </c>
+      <c r="Q39">
+        <v>-9.3469999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>56</v>
+      </c>
+      <c r="M40">
+        <v>0.1</v>
+      </c>
+      <c r="N40">
+        <v>-5.3239999999999998</v>
+      </c>
+      <c r="O40">
+        <v>14.242000000000001</v>
+      </c>
+      <c r="P40">
+        <v>-0.188</v>
+      </c>
+      <c r="Q40">
+        <v>-4.415</v>
+      </c>
+    </row>
+    <row r="41" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L41" t="s">
+        <v>56</v>
+      </c>
+      <c r="M41">
+        <v>0.15</v>
+      </c>
+      <c r="N41">
+        <v>-7.1669999999999998</v>
+      </c>
+      <c r="O41">
+        <v>9.5969999999999995</v>
+      </c>
+      <c r="P41">
+        <v>-0.20699999999999999</v>
+      </c>
+      <c r="Q41">
+        <v>-11.026999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>56</v>
+      </c>
+      <c r="M42">
+        <v>0.2</v>
+      </c>
+      <c r="N42">
+        <v>-4.1859999999999999</v>
+      </c>
+      <c r="O42">
+        <v>14.459</v>
+      </c>
+      <c r="P42">
+        <v>-0.18</v>
+      </c>
+      <c r="Q42">
+        <v>-4.74</v>
+      </c>
+    </row>
+    <row r="43" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>56</v>
+      </c>
+      <c r="M43">
+        <v>0.25</v>
+      </c>
+      <c r="N43">
+        <v>-4.9409999999999998</v>
+      </c>
+      <c r="O43">
+        <v>9.6340000000000003</v>
+      </c>
+      <c r="P43">
+        <v>-0.19700000000000001</v>
+      </c>
+      <c r="Q43">
+        <v>-10.942</v>
+      </c>
+    </row>
+    <row r="44" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>56</v>
+      </c>
+      <c r="M44">
+        <v>0.3</v>
+      </c>
+      <c r="N44">
+        <v>-4.6120000000000001</v>
+      </c>
+      <c r="O44">
+        <v>9.6549999999999994</v>
+      </c>
+      <c r="P44">
+        <v>-0.192</v>
+      </c>
+      <c r="Q44">
+        <v>-10.894</v>
+      </c>
+    </row>
+    <row r="45" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>56</v>
+      </c>
+      <c r="M45">
+        <v>0.35</v>
+      </c>
+      <c r="N45">
+        <v>-6.76</v>
+      </c>
+      <c r="O45">
+        <v>9.6760000000000002</v>
+      </c>
+      <c r="P45">
+        <v>-0.187</v>
+      </c>
+      <c r="Q45">
+        <v>-10.843999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
+        <v>56</v>
+      </c>
+      <c r="M46">
+        <v>0.4</v>
+      </c>
+      <c r="N46">
+        <v>-4.8230000000000004</v>
+      </c>
+      <c r="O46">
+        <v>15.039</v>
+      </c>
+      <c r="P46">
+        <v>-0.16200000000000001</v>
+      </c>
+      <c r="Q46">
+        <v>-5.6289999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A7:G27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>7.5</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>12.5</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>17.5</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>0.68159999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.74770000000000003</v>
+      </c>
+      <c r="D9">
+        <v>0.78920000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.78139999999999998</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>B9*$C$7</f>
+        <v>477.12</v>
+      </c>
+      <c r="C10">
+        <f>C9*$C$7</f>
+        <v>523.39</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:G10" si="0">D9*$C$7</f>
+        <v>552.44000000000005</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>546.98</v>
+      </c>
+      <c r="F10" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G10" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7.5</v>
+      </c>
+      <c r="B14">
+        <v>-1.1839999999999999</v>
+      </c>
+      <c r="C14">
+        <v>13.64</v>
+      </c>
+      <c r="D14">
+        <v>-0.17100000000000001</v>
+      </c>
+      <c r="E14">
+        <v>-10.045999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>-0.877</v>
+      </c>
+      <c r="C15">
+        <v>9.5250000000000004</v>
+      </c>
+      <c r="D15">
+        <v>-0.17</v>
+      </c>
+      <c r="E15">
+        <v>-10.196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12.5</v>
+      </c>
+      <c r="B16">
+        <v>-0.88600000000000001</v>
+      </c>
+      <c r="C16">
+        <v>9.5960000000000001</v>
+      </c>
+      <c r="D16">
+        <v>-0.17</v>
+      </c>
+      <c r="E16">
+        <v>-10.247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>-1.121</v>
+      </c>
+      <c r="C17">
+        <v>13.638</v>
+      </c>
+      <c r="D17">
+        <v>-0.17299999999999999</v>
+      </c>
+      <c r="E17">
+        <v>-10.134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17.5</v>
+      </c>
+      <c r="B18">
+        <v>-0.27300000000000002</v>
+      </c>
+      <c r="C18">
+        <v>9.4809999999999999</v>
+      </c>
+      <c r="D18">
+        <v>-0.17100000000000001</v>
+      </c>
+      <c r="E18">
+        <v>-10.215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>-0.22900000000000001</v>
+      </c>
+      <c r="C19">
+        <v>12.686</v>
+      </c>
+      <c r="D19">
+        <v>-0.17100000000000001</v>
+      </c>
+      <c r="E19">
+        <v>-8.8480000000000008</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3285,25 +6113,164 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
-        <v>41</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7.5</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.12</v>
+      </c>
+      <c r="E22">
+        <v>-11.586</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.121</v>
+      </c>
+      <c r="E23">
+        <v>-9.8309999999999995</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>12.5</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.123</v>
+      </c>
+      <c r="E24">
+        <v>-10.051</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.124</v>
+      </c>
+      <c r="E25">
+        <v>-11.677</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>17.5</v>
+      </c>
+      <c r="B26">
+        <v>1.65</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="E26">
+        <v>-4.1689999999999996</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0.56799999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0.128</v>
+      </c>
+      <c r="E27">
+        <v>-1.4330000000000001</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1.026</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A lot of new changes
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="lattice" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="105">
   <si>
     <t xml:space="preserve">Number of unit cells in spanwise direction </t>
   </si>
@@ -328,6 +328,15 @@
   </si>
   <si>
     <t>Wide</t>
+  </si>
+  <si>
+    <t>Wider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cd </t>
+  </si>
+  <si>
+    <t>wide</t>
   </si>
 </sst>
 </file>
@@ -488,11 +497,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72441856"/>
-        <c:axId val="72442432"/>
+        <c:axId val="66844864"/>
+        <c:axId val="66845440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72441856"/>
+        <c:axId val="66844864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -539,12 +548,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72442432"/>
+        <c:crossAx val="66845440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72442432"/>
+        <c:axId val="66845440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200"/>
@@ -586,7 +595,229 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72441856"/>
+        <c:crossAx val="66844864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_r!$H$8:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_r!$H$10:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>495.90000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>516.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>670.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>696.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>778.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="110994560"/>
+        <c:axId val="110995136"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="110994560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Chiral node</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> radius (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="110995136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="110995136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="800"/>
+          <c:min val="400"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="110994560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -678,11 +909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72444160"/>
-        <c:axId val="72444736"/>
+        <c:axId val="118112832"/>
+        <c:axId val="118113408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72444160"/>
+        <c:axId val="118112832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,12 +923,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72444736"/>
+        <c:crossAx val="118113408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72444736"/>
+        <c:axId val="118113408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -708,7 +939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72444160"/>
+        <c:crossAx val="118112832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -844,14 +1075,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95109696"/>
-        <c:axId val="72559424"/>
+        <c:axId val="118115136"/>
+        <c:axId val="118115712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95109696"/>
+        <c:axId val="118115136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.1"/>
+          <c:max val="8.0000000000000016E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -894,12 +1125,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72559424"/>
+        <c:crossAx val="118115712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72559424"/>
+        <c:axId val="118115712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="400"/>
@@ -941,7 +1172,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95109696"/>
+        <c:crossAx val="118115136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1004,51 +1235,66 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>para_N!$J$8:$O$8</c:f>
+              <c:f>para_eccen!$P$7:$W$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>611.88229999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>713.86699999999996</c:v>
+                  <c:v>5.0000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>815.84</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>917.82</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1019.8</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1121.78</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>para_N!$C$10:$G$10</c:f>
+              <c:f>para_eccen!$P$9:$W$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>522.83000000000004</c:v>
+                  <c:v>509.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>390.53</c:v>
+                  <c:v>511.18899999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>376.74</c:v>
+                  <c:v>486.57000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>333.2</c:v>
+                  <c:v>491.54</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>303.94</c:v>
+                  <c:v>514.08000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>489.92999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>519.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1063,11 +1309,459 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72446464"/>
-        <c:axId val="72447040"/>
+        <c:axId val="120338624"/>
+        <c:axId val="120339200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72446464"/>
+        <c:axId val="120338624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5.000000000000001E-3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Chiral eccentricity (-)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="120339200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="120339200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="400"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="120338624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_B!$F$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_B!$F$10:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>411.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>480.34000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>522.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>557.13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>619.43000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>679</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64294272"/>
+        <c:axId val="64297728"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64294272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="45"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Chiral</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> node depth (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64297728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64297728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="700"/>
+          <c:min val="400"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64294272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_N!$J$8:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>611.88229999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>713.86699999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>815.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>917.82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1019.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1121.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_N!$C$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>522.83000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>390.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>376.74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>333.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>303.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="118117440"/>
+        <c:axId val="118118016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="118117440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1100"/>
@@ -1122,12 +1816,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72447040"/>
+        <c:crossAx val="118118016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72447040"/>
+        <c:axId val="118118016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1170,578 +1864,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72446464"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>para_chiral_t!$F$8:$S$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>para_chiral_t!$F$10:$S$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>126</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>156.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>200.48</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>222.25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>264.18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>295.46999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>331.31</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>476.84000000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>456.40000000000003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>544.53</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>598.99</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>620.54999999999995</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>652.89</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>689.40199999999993</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="72448768"/>
-        <c:axId val="72449344"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="72448768"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="0.4"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="15875"/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Chiral lattice</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                  <a:t> thickness </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>(mm)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="72449344"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="72449344"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="200"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Force (N)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="72448768"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>para_chiral_t!$M$32:$M$46</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.35</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>para_chiral_t!$N$32:$N$46</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>-5.35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-10.475</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-4.9169999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.247</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-3.4420000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-5.3710000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-4.0330000000000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.379</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-5.3239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-7.1669999999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-4.1859999999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-4.9409999999999998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-4.6120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-6.76</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-4.8230000000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="94282880"/>
-        <c:axId val="94283456"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="94282880"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="15875"/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Chiral lattice</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                  <a:t> thickness </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>(mm)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="94283456"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="94283456"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="el-GR" sz="1400">
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>ϕ</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="es-ES" sz="1400" baseline="-25000">
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>tip</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t> (deg)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="94282880"/>
+        <c:crossAx val="118117440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1804,42 +1927,102 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>para_r!$B$8:$E$8</c:f>
+              <c:f>para_chiral_t!$F$8:$S$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>7.5</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.5</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>para_r!$B$10:$E$10</c:f>
+              <c:f>para_chiral_t!$F$10:$S$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>477.12</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>523.39</c:v>
+                  <c:v>156.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>552.44000000000005</c:v>
+                  <c:v>200.48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>546.98</c:v>
+                  <c:v>222.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>264.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>295.46999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>331.31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>476.84000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>456.40000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>544.53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>598.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>620.54999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>652.89</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>689.40199999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1854,11 +2037,522 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94285184"/>
-        <c:axId val="94285760"/>
+        <c:axId val="118119744"/>
+        <c:axId val="118513664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94285184"/>
+        <c:axId val="118119744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Chiral lattice</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> thickness </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>(mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="118513664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="118513664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="118119744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_chiral_t!$M$32:$M$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_chiral_t!$N$32:$N$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-5.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10.475</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.9169999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.247</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.4420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.3710000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.0330000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.379</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.3239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-7.1669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.1859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.9409999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.6120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-6.76</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.8230000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="118515392"/>
+        <c:axId val="118515968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="118515392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Chiral lattice</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> thickness </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>(mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="118515968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="118515968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1400">
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>ϕ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" sz="1400" baseline="-25000">
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>tip</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t> (deg)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="118515392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>para_r!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>para_r!$B$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>477.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>523.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>552.44000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>546.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="118517696"/>
+        <c:axId val="118518272"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="118517696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1911,12 +2605,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94285760"/>
+        <c:crossAx val="118518272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94285760"/>
+        <c:axId val="118518272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1957,7 +2651,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94285184"/>
+        <c:crossAx val="118517696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2044,15 +2738,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>240846</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>421822</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2073,10 +2767,79 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2113,7 +2876,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2149,16 +2912,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>134471</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>312645</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>20171</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>379880</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2182,19 +2945,19 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>517072</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>312644</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>217395</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2211,6 +2974,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>231320</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3534,10 +4329,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S93"/>
+  <dimension ref="A1:W118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3545,38 +4340,22 @@
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0.8</v>
       </c>
-      <c r="S3" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S4" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S5" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -3589,11 +4368,14 @@
       <c r="H6">
         <v>700</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -3639,11 +4421,32 @@
       <c r="O7">
         <v>0.12</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="R7">
+        <v>1E-3</v>
+      </c>
+      <c r="S7">
+        <v>1.5E-3</v>
+      </c>
+      <c r="T7">
+        <v>2E-3</v>
+      </c>
+      <c r="U7">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="V7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="W7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -3689,11 +4492,32 @@
       <c r="O8" t="s">
         <v>28</v>
       </c>
-      <c r="S8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>0.72770000000000001</v>
+      </c>
+      <c r="Q8">
+        <v>0.73026999999999997</v>
+      </c>
+      <c r="R8">
+        <v>0.69510000000000005</v>
+      </c>
+      <c r="S8">
+        <v>0.70220000000000005</v>
+      </c>
+      <c r="T8">
+        <v>0.73440000000000005</v>
+      </c>
+      <c r="U8">
+        <v>0.73180000000000001</v>
+      </c>
+      <c r="V8">
+        <v>0.69989999999999997</v>
+      </c>
+      <c r="W8">
+        <v>0.74160000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G9">
         <f>G8*$H$6</f>
         <v>509.66999999999996</v>
@@ -3722,24 +4546,45 @@
         <f t="shared" si="0"/>
         <v>662.06</v>
       </c>
-      <c r="S9" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S10" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <f>P8*$Q$6</f>
+        <v>509.39</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ref="Q9:V9" si="1">Q8*$Q$6</f>
+        <v>511.18899999999996</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>486.57000000000005</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="1"/>
+        <v>491.54</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>514.08000000000004</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="1"/>
+        <v>512.26</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="1"/>
+        <v>489.92999999999995</v>
+      </c>
+      <c r="W9">
+        <f>W8*$Q$6</f>
+        <v>519.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="S11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -3755,11 +4600,8 @@
       <c r="E12" t="s">
         <v>94</v>
       </c>
-      <c r="S12" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -3775,11 +4617,8 @@
       <c r="E13">
         <v>-10.14</v>
       </c>
-      <c r="S13" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1E-3</v>
       </c>
@@ -3795,11 +4634,8 @@
       <c r="E14">
         <v>-9.9309999999999992</v>
       </c>
-      <c r="S14" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.01</v>
       </c>
@@ -3815,11 +4651,8 @@
       <c r="E15">
         <v>-10.196</v>
       </c>
-      <c r="S15" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.05</v>
       </c>
@@ -3835,11 +4668,8 @@
       <c r="E16">
         <v>-10.598000000000001</v>
       </c>
-      <c r="S16" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.1</v>
       </c>
@@ -3855,24 +4685,13 @@
       <c r="E17">
         <v>-10.601000000000001</v>
       </c>
-      <c r="S17" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S18" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="S19" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -3894,11 +4713,8 @@
       <c r="G20" t="s">
         <v>98</v>
       </c>
-      <c r="S20" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -3920,11 +4736,8 @@
       <c r="G21">
         <v>0.33400000000000002</v>
       </c>
-      <c r="S21" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1E-3</v>
       </c>
@@ -3946,11 +4759,8 @@
       <c r="G22">
         <v>0.33400000000000002</v>
       </c>
-      <c r="S22" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.01</v>
       </c>
@@ -3972,11 +4782,8 @@
       <c r="G23">
         <v>0.33400000000000002</v>
       </c>
-      <c r="S23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.05</v>
       </c>
@@ -3998,11 +4805,8 @@
       <c r="G24">
         <v>0.33400000000000002</v>
       </c>
-      <c r="S24" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.1</v>
       </c>
@@ -4015,347 +4819,467 @@
       <c r="G25">
         <v>0.97099999999999997</v>
       </c>
-      <c r="S25" s="2">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>8</v>
+      </c>
+      <c r="W38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S26" s="2" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S27" s="2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S28" s="2" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S29" s="2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S30" s="2" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S31" s="2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S32" s="2" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S33" s="2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S34" s="2" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S35" s="2" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S36" s="2" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S37" s="2" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S38" s="2" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S39" s="2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S40" s="2" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S41" s="2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S42" s="2" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S43" s="2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
         <v>713.86273190300005</v>
       </c>
     </row>
-    <row r="44" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S44" s="2" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S45" s="2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="46" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S46" s="2" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S47" s="2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S48" s="2" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S49" s="2" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S50" s="2" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S51" s="2" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S52" s="2" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S53" s="2" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S54" s="2" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S55" s="2" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S56" s="2" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S57" s="2" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S58" s="2" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S59" s="2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
         <v>-50</v>
       </c>
     </row>
-    <row r="60" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S60" s="2" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S61" s="2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
         <v>-700</v>
       </c>
     </row>
-    <row r="62" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S62" s="2" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S63" s="2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
         <v>-200000</v>
       </c>
     </row>
-    <row r="64" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S64" s="2" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S65" s="2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="66" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S66" s="2" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S67" s="2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S68" s="2" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S69" s="2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S70" s="2" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S71" s="2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S72" s="2" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S73" s="2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S74" s="2" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S75" s="2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S76" s="2" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S77" s="2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="78" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S78" s="2" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S79" s="2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="80" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S80" s="2" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S81" s="3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
         <v>1.0000000000000001E-15</v>
       </c>
     </row>
-    <row r="82" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S82" s="2" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S83" s="2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="84" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S84" s="2" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S85" s="2" t="b">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S86" s="2" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S87" s="2" t="b">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S88" s="2" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S89" s="3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
         <v>2E-8</v>
       </c>
     </row>
-    <row r="90" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S90" s="2" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S91" s="2" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="92" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S92" s="2" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S93" s="2" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4367,10 +5291,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:G24"/>
+  <dimension ref="A7:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4378,15 +5302,21 @@
     <col min="1" max="1" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="C7">
         <v>-700</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4399,8 +5329,32 @@
       <c r="D8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>25</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>40</v>
+      </c>
+      <c r="L8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4413,13 +5367,64 @@
       <c r="D9">
         <v>0.85980000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>0.61360000000000003</v>
+      </c>
+      <c r="F9">
+        <v>0.58840000000000003</v>
+      </c>
+      <c r="G9">
+        <v>0.68620000000000003</v>
+      </c>
+      <c r="H9">
+        <v>0.747</v>
+      </c>
+      <c r="I9">
+        <v>0.79590000000000005</v>
+      </c>
+      <c r="J9">
+        <v>0.88490000000000002</v>
+      </c>
+      <c r="K9">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>E9*$F$7</f>
+        <v>429.52000000000004</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10:K10" si="0">F9*$F$7</f>
+        <v>411.88</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>480.34000000000003</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>522.9</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>557.13</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>619.43000000000006</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -4436,7 +5441,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -4453,7 +5458,7 @@
         <v>-10.614000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -4470,7 +5475,7 @@
         <v>-10.196</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>30</v>
       </c>
@@ -4586,6 +5591,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5286,7 +6292,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:H24"/>
+  <dimension ref="A7:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N32" sqref="N32"/>
@@ -5297,15 +6303,18 @@
     <col min="1" max="1" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="C7">
         <v>-700</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -5319,7 +6328,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5327,12 +6336,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -5349,82 +6358,55 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>30</v>
       </c>
       <c r="B14">
-        <v>-0.159</v>
+        <v>-0.16200000000000001</v>
       </c>
       <c r="C14">
-        <v>14.946999999999999</v>
+        <v>11.739000000000001</v>
       </c>
       <c r="D14">
-        <v>-0.126</v>
+        <v>-0.124</v>
       </c>
       <c r="E14">
-        <v>-15.25</v>
-      </c>
-      <c r="F14">
-        <v>-0.999</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0.60199999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-9.4410000000000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>50</v>
       </c>
       <c r="B15">
-        <v>-10.946</v>
+        <v>-0.877</v>
       </c>
       <c r="C15">
-        <v>13.666</v>
+        <v>9.5250000000000004</v>
       </c>
       <c r="D15">
-        <v>-0.17499999999999999</v>
+        <v>-0.17</v>
       </c>
       <c r="E15">
-        <v>-10.269</v>
-      </c>
-      <c r="F15">
-        <v>-122.756</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0.54600000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-10.196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
       <c r="B16">
-        <v>-14.752000000000001</v>
+        <v>-4.3739999999999997</v>
       </c>
       <c r="C16">
-        <v>8.6950000000000003</v>
+        <v>8.5630000000000006</v>
       </c>
       <c r="D16">
-        <v>-0.20799999999999999</v>
+        <v>-0.20499999999999999</v>
       </c>
       <c r="E16">
-        <v>-10.125999999999999</v>
-      </c>
-      <c r="F16">
-        <v>-99.478999999999999</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>0.46300000000000002</v>
+        <v>-9.9149999999999991</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5468,6 +6450,15 @@
       <c r="D22">
         <v>7.4999999999999997E-2</v>
       </c>
+      <c r="E22">
+        <v>-1.032</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.60199999999999998</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -5482,6 +6473,15 @@
       <c r="D23">
         <v>0.121</v>
       </c>
+      <c r="E23">
+        <v>-9.8309999999999995</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.33400000000000002</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -5495,6 +6495,15 @@
       </c>
       <c r="D24">
         <v>0.16800000000000001</v>
+      </c>
+      <c r="E24">
+        <v>-27.936</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0.46300000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -5506,8 +6515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:V46"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6239,10 +7248,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:G27"/>
+  <dimension ref="A7:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:H19"/>
+    <sheetView topLeftCell="B2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6250,15 +7259,21 @@
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="C7">
         <v>700</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -6280,8 +7295,23 @@
       <c r="G8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>7.5</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>12.5</v>
+      </c>
+      <c r="K8">
+        <v>15</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -6303,8 +7333,23 @@
       <c r="G9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>0.49590000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.51649999999999996</v>
+      </c>
+      <c r="J9">
+        <v>0.67049999999999998</v>
+      </c>
+      <c r="K9">
+        <v>0.69679999999999997</v>
+      </c>
+      <c r="L9">
+        <v>0.77829999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>B9*$C$7</f>
         <v>477.12</v>
@@ -6329,13 +7374,33 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f>H9*$I$7</f>
+        <v>495.90000000000003</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10:L10" si="1">I9*$I$7</f>
+        <v>516.5</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>670.5</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>696.8</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>778.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -6352,7 +7417,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7.5</v>
       </c>
@@ -6369,7 +7434,7 @@
         <v>-10.045999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -6386,7 +7451,7 @@
         <v>-10.196</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12.5</v>
       </c>

</xml_diff>